<commit_message>
Updating some text in my sections. Updating Schedule
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kyle.cornwall\000TempNotebookHolder\Final Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37877914-DBE9-4847-B620-5D100B255015}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C33DB486-6D3F-4A00-933F-C34CD3DF74D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="64575" yWindow="6975" windowWidth="43200" windowHeight="23535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GANTT" sheetId="1" r:id="rId1"/>
@@ -96,12 +96,6 @@
     <t>Linear Regression Interpretation</t>
   </si>
   <si>
-    <t>Decision Tree Creation</t>
-  </si>
-  <si>
-    <t>Decision Tree Interpretation</t>
-  </si>
-  <si>
     <t>Finalization Phase</t>
   </si>
   <si>
@@ -127,6 +121,12 @@
   </si>
   <si>
     <t>TBD</t>
+  </si>
+  <si>
+    <t>Decision Tree/Random Forest Creation</t>
+  </si>
+  <si>
+    <t>Decision Tree/Random Forest Interpretation</t>
   </si>
 </sst>
 </file>
@@ -836,7 +836,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
+      <selection pane="bottomLeft" activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1006,7 +1006,7 @@
         <v>7</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E7" s="9" t="s">
         <v>8</v>
@@ -1033,7 +1033,7 @@
         <v>7</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E8" s="9" t="s">
         <v>8</v>
@@ -1062,7 +1062,7 @@
         <v>7</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E9" s="9" t="s">
         <v>8</v>
@@ -1125,7 +1125,7 @@
         <v>7</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E12" s="9" t="s">
         <v>8</v>
@@ -1152,7 +1152,7 @@
         <v>7</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E13" s="9" t="s">
         <v>8</v>
@@ -1171,7 +1171,7 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="37" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B14" s="21">
         <v>43904</v>
@@ -1197,7 +1197,7 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="37" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B15" s="21">
         <v>43904</v>
@@ -1232,7 +1232,7 @@
         <v>7</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E16" s="9"/>
       <c r="F16" s="10"/>
@@ -1258,7 +1258,7 @@
         <v>7</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E17" s="9" t="s">
         <v>8</v>
@@ -1324,7 +1324,7 @@
         <v>7</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E20" s="9" t="s">
         <v>8</v>
@@ -1352,7 +1352,7 @@
         <v>7</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E21" s="9" t="s">
         <v>8</v>
@@ -1371,7 +1371,7 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="41" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="B22" s="21">
         <v>43925</v>
@@ -1380,7 +1380,7 @@
         <v>7</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E22" s="9" t="s">
         <v>8</v>
@@ -1399,7 +1399,7 @@
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="41" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="B23" s="21">
         <v>43925</v>
@@ -1408,7 +1408,7 @@
         <v>7</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E23" s="9" t="s">
         <v>8</v>
@@ -1447,7 +1447,7 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="40" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
@@ -1467,7 +1467,7 @@
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="46" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B26" s="21">
         <v>43932</v>
@@ -1495,7 +1495,7 @@
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="46" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B27" s="21">
         <v>43939</v>

</xml_diff>